<commit_message>
Função criar novo personagem finalizada
</commit_message>
<xml_diff>
--- a/Fichas dos personagens.xlsx
+++ b/Fichas dos personagens.xlsx
@@ -1,38 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcos\Desktop\PROJETO GURPS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F0D4E07-8FBF-4919-B0D4-EF97F8D5183D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Temp" sheetId="1" r:id="rId1"/>
+    <sheet name="Temp" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Temporário" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -51,21 +47,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -353,13 +408,540 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nome: </t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Player: </t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total de pontos: </t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total de desvantagens: </t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">XP guardado: </t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr"/>
+      <c r="C6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ST: </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>valorst</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>xpst</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DX: </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>valordx</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>xpdx</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IQ: </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>valoriq</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>xpiq</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HT: </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>valorht</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>xpht</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HP: </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>valorhp</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FP: </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>valorfp</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Swing: </t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>valorsw</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thrusting: </t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>valorthr</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>d6</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Basic Lift(lbs/kg)</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>valor</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>lbs</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>valor</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Encumbrance: </t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>valorencumbrance</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RD: </t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>vamorrd</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic Speed: </t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>vamorbs</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basic Move: </t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>valorbm</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>m/s</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="inlineStr"/>
+      <c r="C24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Will: </t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>valorwill</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Per:</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>valorpercepção</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Stress: </t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>valorstress</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="inlineStr"/>
+      <c r="C28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dodge: </t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>valordodge</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parry weapon: </t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>valorparryw</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Parry unarmed: </t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>valorparryu</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="inlineStr"/>
+      <c r="C32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ADVANTAGE </t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>xpvantagens</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>nomevantagem</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>xpvantagem</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr"/>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DISADVANTAGE </t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr"/>
+      <c r="B39" t="inlineStr"/>
+      <c r="C39" t="inlineStr"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr"/>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SKILLS </t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>xpskill</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>C</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>NH</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>nome</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>custo</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>/</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>nh</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+      <c r="B43" t="inlineStr"/>
+      <c r="C43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr"/>
+      <c r="B44" t="inlineStr"/>
+      <c r="C44" t="inlineStr"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BACKGROUND: </t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>história do personagemaqui</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Criação e início da implementação das mensagens do sistema
</commit_message>
<xml_diff>
--- a/Fichas dos personagens.xlsx
+++ b/Fichas dos personagens.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Temp" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Temporário" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Temporário1" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -944,4 +945,22 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Correções dos calculos de Atributos
</commit_message>
<xml_diff>
--- a/Fichas dos personagens.xlsx
+++ b/Fichas dos personagens.xlsx
@@ -1,14 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <workbookPr/>
+  <workbookPr codeName="EstaPastaDeTrabalho"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-18420" yWindow="375" windowWidth="16470" windowHeight="10305" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="----------PERSONAGENS----------" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Zai Kyeroshi - Marcos" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Teste - Marcos" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Personagem Teste - Marcos" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -410,13 +409,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+  <sheetPr codeName="Planilha1">
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:A1"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
@@ -434,446 +433,6 @@
   </sheetPr>
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Nome: </t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Player: </t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Total de pontos: </t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Total de desvantagens: </t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t xml:space="preserve">XP guardado: </t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ST: </t>
-        </is>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DX: </t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">IQ: </t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t xml:space="preserve">HT: </t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t xml:space="preserve">HP: </t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FP: </t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Swing: </t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>d6</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Thrusting: </t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>d6</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Basic Lift(lbs/kg)</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>valor</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>lbs</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>valor</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>kg</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Encumbrance: </t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>valorencumbrance</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t xml:space="preserve">RD: </t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>vamorrd</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Basic Speed: </t>
-        </is>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>vamorbs</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Basic Move: </t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>valorbm</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>m/s</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Will: </t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>valorwill</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Per:</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>valorpercepção</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Stress: </t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>valorstress</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Dodge: </t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>valordodge</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parry weapon: </t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>valorparryw</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Parry unarmed: </t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>valorparryu</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ADVANTAGE </t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>xpvantagens</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>nomevantagem</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>xpvantagem</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t xml:space="preserve">DISADVANTAGE </t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SKILLS </t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>xpskill</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>C</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>NH</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>nome</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>custo</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>/</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>nh</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t xml:space="preserve">BACKGROUND: </t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>história do personagemaqui</t>
-        </is>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F46"/>
-  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
@@ -913,6 +472,8 @@
         </is>
       </c>
     </row>
+    <row r="5"/>
+    <row r="6"/>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
@@ -920,10 +481,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C7" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -932,15 +493,11 @@
           <t xml:space="preserve">DX: </t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B8" t="n">
+        <v>12</v>
+      </c>
+      <c r="C8" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -949,15 +506,11 @@
           <t xml:space="preserve">IQ: </t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="B9" t="n">
+        <v>13</v>
+      </c>
+      <c r="C9" t="n">
+        <v>60</v>
       </c>
     </row>
     <row r="10">
@@ -966,17 +519,15 @@
           <t xml:space="preserve">HT: </t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-    </row>
+      <c r="B10" t="n">
+        <v>18</v>
+      </c>
+      <c r="C10" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11"/>
+    <row r="12"/>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
@@ -1001,6 +552,7 @@
         </is>
       </c>
     </row>
+    <row r="15"/>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
@@ -1101,6 +653,7 @@
         </is>
       </c>
     </row>
+    <row r="21"/>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
@@ -1130,6 +683,7 @@
         </is>
       </c>
     </row>
+    <row r="24"/>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
@@ -1171,6 +725,7 @@
         </is>
       </c>
     </row>
+    <row r="28"/>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
@@ -1207,6 +762,8 @@
         </is>
       </c>
     </row>
+    <row r="32"/>
+    <row r="33"/>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
@@ -1231,6 +788,8 @@
         </is>
       </c>
     </row>
+    <row r="36"/>
+    <row r="37"/>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
@@ -1238,6 +797,8 @@
         </is>
       </c>
     </row>
+    <row r="39"/>
+    <row r="40"/>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
@@ -1287,6 +848,8 @@
         </is>
       </c>
     </row>
+    <row r="43"/>
+    <row r="44"/>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>

</xml_diff>